<commit_message>
tests done using testNg
</commit_message>
<xml_diff>
--- a/com.luma/src/test/resources/test_data.xlsx
+++ b/com.luma/src/test/resources/test_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="90" windowWidth="12420" windowHeight="3590" activeTab="3"/>
+    <workbookView xWindow="80" yWindow="90" windowWidth="12420" windowHeight="3590" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="doSignIn" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,6 @@
     <sheet name="doSubscribe" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -105,51 +104,15 @@
     <t>kenza</t>
   </si>
   <si>
-    <t>lindsey</t>
-  </si>
-  <si>
-    <t>kenzo</t>
-  </si>
-  <si>
     <t>Ken@278!</t>
   </si>
   <si>
-    <t>Lind@12#</t>
-  </si>
-  <si>
-    <t>lilise</t>
-  </si>
-  <si>
     <t>lysa</t>
   </si>
   <si>
-    <t>Lysa96@%!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">katia </t>
-  </si>
-  <si>
     <t>kate</t>
   </si>
   <si>
-    <t>Kati93@!&amp;19</t>
-  </si>
-  <si>
-    <t>lindalydo@gmail.com</t>
-  </si>
-  <si>
-    <t>kenza23@gmail.com</t>
-  </si>
-  <si>
-    <t>lysalysa@gmail.com</t>
-  </si>
-  <si>
-    <t>katykatia@gmail.com</t>
-  </si>
-  <si>
-    <t>Fazia@19096us</t>
-  </si>
-  <si>
     <t>faz1996@gmail.com</t>
   </si>
   <si>
@@ -160,6 +123,42 @@
   </si>
   <si>
     <t>fazo93@gmail.com</t>
+  </si>
+  <si>
+    <t>Fazia@96us</t>
+  </si>
+  <si>
+    <t>katou</t>
+  </si>
+  <si>
+    <t>katekatrine@gmail.com</t>
+  </si>
+  <si>
+    <t>Kati1993@!&amp;19</t>
+  </si>
+  <si>
+    <t>lulu</t>
+  </si>
+  <si>
+    <t>lysa.llulu92@gmail.com</t>
+  </si>
+  <si>
+    <t>Lysa916@%!</t>
+  </si>
+  <si>
+    <t>keran</t>
+  </si>
+  <si>
+    <t>kenza2023@gmail.com</t>
+  </si>
+  <si>
+    <t>lady</t>
+  </si>
+  <si>
+    <t>linda.laydo@gmail.com</t>
+  </si>
+  <si>
+    <t>Lind@1212#</t>
   </si>
 </sst>
 </file>
@@ -531,7 +530,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="29">
@@ -665,8 +664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -694,13 +693,13 @@
         <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -708,41 +707,41 @@
         <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
         <v>36</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -765,7 +764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -778,22 +777,22 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>